<commit_message>
ANV - 20220330 - Updated code
</commit_message>
<xml_diff>
--- a/TH02/Variation Data/TH02.xlsx
+++ b/TH02/Variation Data/TH02.xlsx
@@ -69,7 +69,7 @@
     <x:t>Se positionner sur la date d'application à la cession</x:t>
   </x:si>
   <x:si>
-    <x:t>34</x:t>
+    <x:t>45</x:t>
   </x:si>
   <x:si>
     <x:t>36</x:t>
@@ -166,7 +166,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="7">
+  <x:cellStyleXfs count="10">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -179,6 +179,15 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -531,7 +540,7 @@
       <x:selection activeCell="G2" sqref="G2 G2:G2"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="10.307969" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:sheetFormatPr defaultColWidth="12.439844" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
     <x:col min="1" max="1" width="13.441406" style="4" bestFit="1" customWidth="1"/>
     <x:col min="2" max="3" width="12.21875" style="4" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
ANV 20220330   Chnage in inputfile
</commit_message>
<xml_diff>
--- a/TH02/Variation Data/TH02.xlsx
+++ b/TH02/Variation Data/TH02.xlsx
@@ -5,12 +5,12 @@
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansverma\Desktop\Desktop\Project\ADEO_Laptop29_6_21\Adeo\Project\ISOCEL\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansverma\Desktop\Desktop\Project\ADEO_Laptop29_6_21\Adeo\Project\ISOCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10EA0A1-24F8-4488-9FF1-F74BE03BF72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1067D9C-1D34-423F-BD4C-D9C20E987009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="010_Create_dossier_d'offre" sheetId="2" r:id="rId1"/>
@@ -63,16 +63,16 @@
     <x:t>114213 - L ARTISAN GIVRE</x:t>
   </x:si>
   <x:si>
+    <x:t>274,279,281</x:t>
+  </x:si>
+  <x:si>
     <x:t>Code</x:t>
   </x:si>
   <x:si>
     <x:t>Se positionner sur la date d'application à la cession</x:t>
   </x:si>
   <x:si>
-    <x:t>45</x:t>
-  </x:si>
-  <x:si>
-    <x:t>36</x:t>
+    <x:t>47</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -166,13 +166,13 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="10">
+  <x:cellStyleXfs count="8">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="3" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -181,39 +181,36 @@
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="8">
+  <x:cellXfs count="11">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment wrapText="1"/>
     </x:xf>
-    <x:xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    <x:xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -536,64 +533,64 @@
   </x:sheetPr>
   <x:dimension ref="A1:G2"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
+    <x:sheetView tabSelected="1" workbookViewId="0">
       <x:selection activeCell="G2" sqref="G2 G2:G2"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="12.439844" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:sheetFormatPr defaultColWidth="13.82" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
-    <x:col min="1" max="1" width="13.441406" style="4" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="3" width="12.21875" style="4" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="23.441406" style="4" bestFit="1" customWidth="1"/>
-    <x:col min="5" max="5" width="21.332031" style="4" bestFit="1" customWidth="1"/>
-    <x:col min="6" max="6" width="10.664062" style="4" bestFit="1" customWidth="1"/>
-    <x:col min="7" max="7" width="10.886719" style="4" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="13.441406" style="7" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="3" width="12.21875" style="7" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="23.441406" style="7" bestFit="1" customWidth="1"/>
+    <x:col min="5" max="5" width="21.332031" style="7" bestFit="1" customWidth="1"/>
+    <x:col min="6" max="6" width="10.664062" style="7" bestFit="1" customWidth="1"/>
+    <x:col min="7" max="7" width="12.554688" style="10" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <x:c r="A1" s="7" t="s">
+      <x:c r="A1" s="8" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="7" t="s">
+      <x:c r="B1" s="8" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="7" t="s">
+      <x:c r="C1" s="8" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="7" t="s">
+      <x:c r="D1" s="8" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="7" t="s">
+      <x:c r="E1" s="8" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="7" t="s">
+      <x:c r="F1" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G1" s="7" t="s">
+      <x:c r="G1" s="9" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:7" customFormat="1" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A2" s="6" t="s">
+      <x:c r="A2" s="1" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="B2" s="6" t="s">
+      <x:c r="B2" s="1" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C2" s="6" t="s">
+      <x:c r="C2" s="1" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D2" s="6" t="s">
+      <x:c r="D2" s="1" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="E2" s="6" t="s">
+      <x:c r="E2" s="1" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="F2" s="6" t="s">
+      <x:c r="F2" s="1" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="G2" s="5" t="n">
-        <x:v>274279281</x:v>
+      <x:c r="G2" s="2" t="s">
+        <x:v>13</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -619,58 +616,52 @@
   </x:sheetPr>
   <x:dimension ref="A1:E2"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="G6" sqref="G6 G6:G6"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="E2" sqref="E2 E2:E2"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
-    <x:col min="1" max="1" width="13.441406" style="4" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="3" width="12.21875" style="4" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="5.332031" style="4" bestFit="1" customWidth="1"/>
-    <x:col min="5" max="5" width="10.886719" style="4" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="13.441406" style="7" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="3" width="12.21875" style="7" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="5.332031" style="7" bestFit="1" customWidth="1"/>
+    <x:col min="5" max="5" width="10.886719" style="7" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <x:c r="A1" s="7" t="s">
+    <x:row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="A1" s="8" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="7" t="s">
+      <x:c r="B1" s="8" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="7" t="s">
+      <x:c r="C1" s="8" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="7" t="s">
+      <x:c r="D1" s="8" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E1" s="8" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A2" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B2" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C2" s="1" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D2" s="1" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E2" s="2" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="E1" s="7" t="s">
-        <x:v>6</x:v>
-      </x:c>
     </x:row>
-    <x:row r="2" spans="1:7" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <x:c r="A2" s="6" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B2" s="6" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="C2" s="6" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="D2" s="6" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="E2" s="5" t="n">
-        <x:v>274279281</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:7">
-      <x:c r="D3" s="4" t="s">
-        <x:v>16</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:7"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -688,18 +679,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -875,18 +866,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4622310D-E04A-4C2A-A41F-E463C8085246}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91F80EF2-C61E-4ACC-AE26-5BAD359D81A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4622310D-E04A-4C2A-A41F-E463C8085246}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>